<commit_message>
Added ReadMe to industry shipment data
</commit_message>
<xml_diff>
--- a/input_data/Industry_Shipments/Other_Countries/Shipments_Copper.xlsx
+++ b/input_data/Industry_Shipments/Other_Countries/Shipments_Copper.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B20FEA-C1CC-48E5-8935-8F652E715309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D806BD5C-B05E-4E59-8631-FBC0600C80E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EU" sheetId="2" r:id="rId1"/>
@@ -24,15 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
-  <si>
-    <t>Spatari - Copper North America</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="42">
   <si>
     <t xml:space="preserve">1987  43%  23%  13%  11%  9% </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ciacci 2017 </t>
   </si>
   <si>
     <t>Urban Mines of Copper: Size and Potential for Recycling in the EU</t>
@@ -132,9 +126,6 @@
     <t xml:space="preserve">Consumer and General Products </t>
   </si>
   <si>
-    <t>. Major end-use application sectors of Cu and related market shares. '</t>
-  </si>
-  <si>
     <t>described as:</t>
   </si>
   <si>
@@ -151,6 +142,15 @@
   </si>
   <si>
     <t>Industrial Machinery and Equipment</t>
+  </si>
+  <si>
+    <t>Spatari et al. (2005) Copper North America</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ciacci et al. 2017 </t>
+  </si>
+  <si>
+    <t>Major end-use application sectors of Cu and related market shares. '</t>
   </si>
 </sst>
 </file>
@@ -200,13 +200,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -943,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72894651-DF8A-4E3F-BA25-F2563F45E953}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1268,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P60"/>
+  <dimension ref="B2:R60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1280,9 +1281,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" t="str">
@@ -1783,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C17">
         <f>[1]Copper_Split!C48</f>
         <v>0</v>
@@ -1821,169 +1823,171 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="K20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="J20" t="s">
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
         <v>4</v>
       </c>
-      <c r="K20" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="G23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
+      <c r="G25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="G24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D25" t="s">
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
         <v>7</v>
       </c>
-      <c r="G25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
         <v>8</v>
       </c>
-      <c r="G26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
         <v>9</v>
       </c>
-      <c r="G27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D28" t="s">
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
         <v>10</v>
       </c>
-      <c r="G28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D29" t="s">
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
         <v>11</v>
       </c>
-      <c r="G29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
         <v>12</v>
       </c>
-      <c r="G30" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
-        <v>14</v>
-      </c>
       <c r="G32" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
         <v>15</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
         <v>18</v>
       </c>
-      <c r="E36" t="s">
-        <v>20</v>
-      </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
         <v>19</v>
       </c>
-      <c r="E37" t="s">
-        <v>21</v>
-      </c>
       <c r="F37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.3">
@@ -2026,7 +2030,7 @@
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D41" s="3">
         <v>0.43</v>
@@ -2067,7 +2071,7 @@
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D42" s="2">
         <v>0.23</v>
@@ -2108,7 +2112,7 @@
     </row>
     <row r="43" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D43" s="2">
         <v>0.13</v>
@@ -2149,7 +2153,7 @@
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D44" s="2">
         <v>0.11</v>
@@ -2190,7 +2194,7 @@
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D45" s="2">
         <v>0.09</v>
@@ -2284,22 +2288,22 @@
     </row>
     <row r="49" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" t="s">
+        <v>36</v>
+      </c>
+      <c r="H49" t="s">
         <v>37</v>
-      </c>
-      <c r="D49" t="s">
-        <v>30</v>
-      </c>
-      <c r="E49" t="s">
-        <v>38</v>
-      </c>
-      <c r="F49" t="s">
-        <v>41</v>
-      </c>
-      <c r="G49" t="s">
-        <v>39</v>
-      </c>
-      <c r="H49" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="50" spans="3:15" x14ac:dyDescent="0.3">

</xml_diff>